<commit_message>
chore: update sim inventory template spreadsheet
</commit_message>
<xml_diff>
--- a/app/SimInvy/templates/sim_inventory_template.xlsx
+++ b/app/SimInvy/templates/sim_inventory_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\evehicles\nayasim\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MCA Project\github\nnx\app\SimInvy\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC27E36-048D-472B-9106-CA72BE2690F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FCB743-7DC2-4047-9051-4FF4A539A2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F0C8A9C-4667-4BBE-9D08-551C82CBF372}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,19 +100,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,32 +427,32 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>